<commit_message>
Bug fix - Create without discovery
Correcting default value for instances where resource created without discovery
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11129"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa_1/GitHub/Inventory-Utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim.s\Documents\GitHub\MockResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="4180" windowWidth="51200" windowHeight="23140" tabRatio="713" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="4185" windowWidth="51195" windowHeight="23145" tabRatio="713" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,12 +68,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,12 +156,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -181,12 +181,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>jibranna</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="141">
   <si>
     <t>Ignore</t>
   </si>
@@ -331,9 +331,6 @@
     <t>FolderPath</t>
   </si>
   <si>
-    <t>v2c</t>
-  </si>
-  <si>
     <t>Sheet used to set attributes on a resource or sub-resource
 Place workbook in C:\CloudShell\DataModel.
 Run SetAttributes.py</t>
@@ -373,9 +370,6 @@
   </si>
   <si>
     <t>logfilename</t>
-  </si>
-  <si>
-    <t>PUBLIC</t>
   </si>
   <si>
     <t>IPAddress02</t>
@@ -461,36 +455,12 @@
     <t>NYC_01</t>
   </si>
   <si>
-    <t>CS_ComputeServer</t>
-  </si>
-  <si>
     <t>GenericServer</t>
   </si>
   <si>
-    <t>110.10.11.101</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
-    <t>Port_01</t>
-  </si>
-  <si>
-    <t>CS_Port</t>
-  </si>
-  <si>
-    <t>GenericServer.ResourcePort</t>
-  </si>
-  <si>
     <t>NYC_02</t>
   </si>
   <si>
-    <t>110.10.11.102</t>
-  </si>
-  <si>
     <t>OS Type</t>
   </si>
   <si>
@@ -504,9 +474,6 @@
   </si>
   <si>
     <t>Location</t>
-  </si>
-  <si>
-    <t>Row 14 Rack 6</t>
   </si>
   <si>
     <t>log level</t>
@@ -668,18 +635,6 @@
     <t>ignored if updating</t>
   </si>
   <si>
-    <t>Eth-01</t>
-  </si>
-  <si>
-    <t>enable01</t>
-  </si>
-  <si>
-    <t>Servers/Dev</t>
-  </si>
-  <si>
-    <t>AMR,x_Dev</t>
-  </si>
-  <si>
     <t>localhost</t>
   </si>
   <si>
@@ -700,12 +655,27 @@
   </si>
   <si>
     <t>Under Power Mgmt</t>
+  </si>
+  <si>
+    <t>CS_GenericResource</t>
+  </si>
+  <si>
+    <t>MockResource</t>
+  </si>
+  <si>
+    <t>MockLab</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>Mock:A0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="34">
     <font>
       <sz val="11"/>
@@ -1573,6 +1543,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="50" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1609,22 +1595,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="50" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1954,7 +1924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -1964,14 +1934,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="143.5" customWidth="1"/>
+    <col min="1" max="1" width="143.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="345.5" customHeight="1">
+    <row r="1" spans="1:1" ht="345.6" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1980,103 +1950,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="11" customWidth="1"/>
     <col min="2" max="2" width="36" style="11" customWidth="1"/>
     <col min="3" max="3" width="0" style="11" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="11"/>
+    <col min="4" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
+    <row r="1" spans="1:3" ht="13.5" thickBot="1">
       <c r="A1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>47</v>
-      </c>
       <c r="C1" s="11" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="12" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>$C:$C</formula1>
     </dataValidation>
   </dataValidations>
@@ -2086,36 +2056,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="12.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.25" customHeight="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" ht="73.349999999999994" customHeight="1">
+      <c r="A1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
@@ -2123,17 +2093,17 @@
         <v>42814</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" ht="12.75">
       <c r="F3" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="13" thickBot="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="13" thickBot="1">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2119,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -2163,7 +2133,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -2177,7 +2147,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2191,7 +2161,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -2202,7 +2172,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -2213,7 +2183,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -2224,7 +2194,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -2235,7 +2205,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -2246,7 +2216,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -2257,10 +2227,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2274,50 +2244,50 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="3" width="7.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="7.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="1" customWidth="1"/>
     <col min="21" max="21" width="12" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="1"/>
+    <col min="22" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="85.25" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+    <row r="1" spans="1:21" ht="85.35" customHeight="1">
+      <c r="A1" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
@@ -2330,234 +2300,138 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="26" customFormat="1" ht="37" thickBot="1">
+    <row r="4" spans="1:21" s="26" customFormat="1" ht="48.75" thickBot="1">
       <c r="A4" s="25" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="T4" s="25" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="26" customFormat="1" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="26" customFormat="1" ht="26.1" customHeight="1" thickBot="1">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="40" t="s">
+      <c r="B5" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="40" t="s">
+      <c r="Q5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="40" t="s">
+      <c r="R5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="T5" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="U5" s="41" t="s">
-        <v>150</v>
+      <c r="S5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>87</v>
+        <v>138</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="B7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>140</v>
-      </c>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="B8" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="B9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>140</v>
-      </c>
+      <c r="I9" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2570,158 +2444,158 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="15" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="49.25" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+    <row r="1" spans="1:18" ht="49.35" customHeight="1">
+      <c r="A1" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="8">
         <v>42815</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="D2" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="13" thickBot="1"/>
-    <row r="4" spans="1:18" ht="13" thickBot="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="12.75" thickBot="1"/>
+    <row r="4" spans="1:18" ht="12.75" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="26" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="42" t="s">
+      <c r="C5" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="H5" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="I5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="J5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="K5" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="L5" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="M5" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="N5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="O5" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="P5" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="Q5" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="42" t="s">
+      <c r="R5" s="30" t="s">
         <v>61</v>
-      </c>
-      <c r="Q5" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="R5" s="42" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1">
         <v>10.15</v>
@@ -2729,10 +2603,10 @@
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1">
         <v>2017.1</v>
@@ -2749,32 +2623,32 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="250" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="250" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="40.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.25" customHeight="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:5" ht="55.35" customHeight="1">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
@@ -2782,15 +2656,15 @@
         <v>42815</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="13.5" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13" thickBot="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2803,82 +2677,82 @@
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="B7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="B9" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
       <c r="B11" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15">
       <c r="B12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15">
       <c r="B13" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
       <c r="B14" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
       <c r="B15" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
@@ -2960,7 +2834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -2970,58 +2844,58 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="A1" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3034,87 +2908,87 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="43" customWidth="1"/>
-    <col min="5" max="6" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="31" customWidth="1"/>
+    <col min="5" max="6" width="33.28515625" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="A1" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="24" customFormat="1" thickBot="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="24" customFormat="1" ht="13.5" thickBot="1">
       <c r="A4" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>134</v>
+        <v>118</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>123</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3122,19 +2996,19 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>135</v>
+        <v>112</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G6">
         <v>3</v>

</xml_diff>